<commit_message>
remoção de resultados de testes não executados
</commit_message>
<xml_diff>
--- a/testes/Alugar_Veiculo_Test_Case.xlsx
+++ b/testes/Alugar_Veiculo_Test_Case.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,15 +18,17 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$1:$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$B$1:$R$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$B$1:$R$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$B$1:$R$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$1:$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$1:$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'UCXXX - &lt;Nome do UC&gt;'!$1:$6</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -227,55 +229,10 @@
 Senha:1234                                               RETIRADA: 29/04/2015</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETORNAR MENSAGEM: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>VEÍCULO ALUGADO</t>
-    </r>
-  </si>
-  <si>
     <t>ALUGAR VEÍCULO SEGUNDO CAMINHO</t>
   </si>
   <si>
     <t>O VISITANTE CLICA EM ALUGAR E PRENCHE OS DADOS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETORNAR MENSAGEM: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>VEÍCULO ALUGADO
-Fluxo alternativo não tratado</t>
-    </r>
   </si>
   <si>
     <t>VISITANTE NÃO LOGADO</t>
@@ -288,9 +245,6 @@
   </si>
   <si>
     <t>O SISTEMA RETORNA A TELA DE LOGIN PARA PREENCHIMENTO DE DADOS</t>
-  </si>
-  <si>
-    <t>Sistema realizando aluguel com dados de acesso na pagina de login</t>
   </si>
   <si>
     <t>LOGIN INCORRETO</t>
@@ -309,28 +263,6 @@
 Senha:12345                                               RETIRADA: 29/04/2015</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETORNA MENSAGEM: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Dados incorretos, verifique seu login e senha</t>
-    </r>
-  </si>
-  <si>
     <t>PRAZO INCORRETO</t>
   </si>
   <si>
@@ -343,28 +275,6 @@
     <t>O SISTEMA RETORNA QUE A DATA É MENOR DO QUE DATA ATUAL</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETORNA MENSAGEM: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Data de aluguel deve ser maior ou igual a data atual</t>
-    </r>
-  </si>
-  <si>
     <t>CT006</t>
   </si>
   <si>
@@ -374,48 +284,7 @@
     <t>O SISTEMA RETORNA QUE A DATA ESTÁ INCONSISTENTE COM A DATA PARA ALUGAR</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETIRADA: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>22/07/2829</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETORNA MENSAGEM: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Data não está de acordo</t>
-    </r>
+    <t>RETIRADA: 22/07/2829</t>
   </si>
   <si>
     <t>CT007</t>
@@ -427,48 +296,7 @@
     <t>O SISTEMA RETORNA QUE PARA O PERÍODO ESCOLHIDO, O VEÍCULO JÁ ESTÁ ALUGADO</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETIRADA: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>15/08/2015</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>RETORNA MENSAGEM: </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Prazo indisponível para aluguel</t>
-    </r>
+    <t>RETIRADA: 15/08/2015</t>
   </si>
   <si>
     <t>CT008</t>
@@ -1343,7 +1171,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1400,516 +1228,12 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="141">
+  <dxfs count="85">
     <dxf>
       <font>
         <name val="Arial"/>
         <charset val="1"/>
         <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFDD0806"/>
       </font>
     </dxf>
     <dxf>
@@ -2745,7 +2069,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3155,7 +2479,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3185,24 +2509,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="25" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="25" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="25" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="25" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="25" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="25" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="25" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="25" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="26" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="27" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="19" style="25" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="23" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="25" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="25" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="25" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="25" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="25" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="25" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="25" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="25" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="26" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="27" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="26" min="19" style="25" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="23" width="3.78061224489796"/>
   </cols>
   <sheetData>
     <row r="1" s="36" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19417,19 +18741,19 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.1632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.484693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19528,11 +18852,9 @@
       <c r="F6" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="98" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="98"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="99"/>
       <c r="B7" s="100"/>
       <c r="C7" s="100"/>
@@ -19546,13 +18868,13 @@
         <v>29</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="95" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="96" t="s">
         <v>64</v>
@@ -19560,11 +18882,9 @@
       <c r="F8" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="98" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="98"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="99"/>
       <c r="B9" s="100"/>
       <c r="C9" s="100"/>
@@ -19578,25 +18898,23 @@
         <v>34</v>
       </c>
       <c r="B10" s="95" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="E10" s="96" t="s">
         <v>71</v>
-      </c>
-      <c r="D10" s="95" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="96" t="s">
-        <v>73</v>
       </c>
       <c r="F10" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="98" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="98"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="99"/>
       <c r="B11" s="101"/>
       <c r="C11" s="100"/>
@@ -19610,25 +18928,23 @@
         <v>42</v>
       </c>
       <c r="B12" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="95" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="95" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="96" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="F12" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="95" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="97" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="98" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="98"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="99"/>
       <c r="B13" s="100"/>
       <c r="C13" s="100"/>
@@ -19642,25 +18958,23 @@
         <v>48</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C14" s="95" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E14" s="96" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F14" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="98" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="98"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="99"/>
       <c r="B15" s="100"/>
       <c r="C15" s="100"/>
@@ -19671,28 +18985,26 @@
     </row>
     <row r="16" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="94" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B16" s="95" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C16" s="95" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D16" s="95" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="96" t="s">
-        <v>88</v>
+      <c r="F16" s="102" t="s">
+        <v>84</v>
       </c>
-      <c r="F16" s="102" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="98" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="98"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="99"/>
       <c r="B17" s="100"/>
       <c r="C17" s="100"/>
@@ -19703,26 +19015,24 @@
     </row>
     <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="94" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C18" s="95" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D18" s="95" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E18" s="96" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F18" s="102" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
-      <c r="G18" s="98" t="s">
-        <v>95</v>
-      </c>
+      <c r="G18" s="98"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="103"/>
@@ -19735,7 +19045,7 @@
     </row>
     <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="94" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B20" s="104"/>
       <c r="C20" s="104"/>
@@ -19755,7 +19065,7 @@
     </row>
     <row r="22" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="94" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B22" s="104"/>
       <c r="C22" s="104"/>
@@ -19775,7 +19085,7 @@
     </row>
     <row r="24" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="94" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B24" s="104"/>
       <c r="C24" s="104"/>
@@ -19795,7 +19105,7 @@
     </row>
     <row r="26" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="94" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B26" s="104"/>
       <c r="C26" s="104"/>
@@ -19815,7 +19125,7 @@
     </row>
     <row r="28" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="94" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B28" s="104"/>
       <c r="C28" s="104"/>
@@ -19835,7 +19145,7 @@
     </row>
     <row r="30" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="94" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B30" s="95"/>
       <c r="C30" s="95"/>
@@ -19855,7 +19165,7 @@
     </row>
     <row r="32" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="94" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B32" s="95"/>
       <c r="C32" s="104"/>
@@ -19875,7 +19185,7 @@
     </row>
     <row r="34" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="94" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B34" s="95"/>
       <c r="C34" s="95"/>
@@ -19895,7 +19205,7 @@
     </row>
     <row r="36" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="94" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B36" s="95"/>
       <c r="C36" s="95"/>
@@ -19915,7 +19225,7 @@
     </row>
     <row r="38" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="94" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B38" s="95"/>
       <c r="C38" s="95"/>
@@ -19935,7 +19245,7 @@
     </row>
     <row r="40" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="94" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B40" s="95"/>
       <c r="C40" s="95"/>
@@ -19955,7 +19265,7 @@
     </row>
     <row r="42" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="94" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B42" s="95"/>
       <c r="C42" s="95"/>
@@ -19975,7 +19285,7 @@
     </row>
     <row r="44" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="94" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B44" s="95"/>
       <c r="C44" s="95"/>
@@ -19995,7 +19305,7 @@
     </row>
     <row r="46" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="94" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B46" s="104"/>
       <c r="C46" s="104"/>
@@ -20009,7 +19319,7 @@
     </row>
     <row r="48" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="94" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B48" s="104"/>
       <c r="C48" s="104"/>
@@ -20023,7 +19333,7 @@
     </row>
     <row r="50" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="94" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B50" s="104"/>
       <c r="C50" s="104"/>
@@ -20037,7 +19347,7 @@
     </row>
     <row r="52" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="94" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B52" s="104"/>
       <c r="C52" s="104"/>
@@ -20051,7 +19361,7 @@
     </row>
     <row r="54" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="94" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B54" s="95"/>
       <c r="C54" s="95"/>
@@ -20065,7 +19375,7 @@
     </row>
     <row r="56" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="94" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B56" s="95"/>
       <c r="C56" s="95"/>
@@ -20079,7 +19389,7 @@
     </row>
     <row r="58" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="94" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B58" s="95"/>
       <c r="C58" s="95"/>
@@ -20093,7 +19403,7 @@
     </row>
     <row r="60" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="94" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B60" s="95"/>
       <c r="C60" s="95"/>
@@ -20104,7 +19414,7 @@
     </row>
     <row r="62" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="94" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B62" s="95"/>
       <c r="C62" s="95"/>
@@ -20118,7 +19428,7 @@
     </row>
     <row r="64" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="94" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B64" s="95"/>
       <c r="C64" s="95"/>
@@ -20132,7 +19442,7 @@
     </row>
     <row r="66" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="94" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B66" s="95"/>
       <c r="C66" s="95"/>

</xml_diff>